<commit_message>
Schablonen cleanup und neue Endo-Schablonen
</commit_message>
<xml_diff>
--- a/Schablonen/Divertikulose.xlsx
+++ b/Schablonen/Divertikulose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F281ADF0-B3B9-40BC-B679-6B1659B3226E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FE9ADF-DE29-435A-BC43-4DBF54BBEBC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61320" yWindow="6690" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="41180" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Textbausteine befundeingabestru" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t>Gliederung</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Text Befund</t>
   </si>
   <si>
-    <t>Aufzählungstexte</t>
-  </si>
-  <si>
     <t>Text Beurteilung</t>
   </si>
   <si>
@@ -92,36 +89,6 @@
     <t>Block</t>
   </si>
   <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
-    <t>einzelne Divertikel</t>
-  </si>
-  <si>
-    <t>mehrere Divertikel</t>
-  </si>
-  <si>
-    <t>einzelne Divertikel;einzeln; einzelne</t>
-  </si>
-  <si>
-    <t>mehrere Divertikel; mehrere</t>
-  </si>
-  <si>
-    <t>viele Divertikel</t>
-  </si>
-  <si>
-    <t>viele Divertikel; viele</t>
-  </si>
-  <si>
-    <t>viele, große Divertikel</t>
-  </si>
-  <si>
-    <t>viele, große Divertikel;viele große Divertikel;viele große;viele, große</t>
-  </si>
-  <si>
-    <t>Hauptlokalisation</t>
-  </si>
-  <si>
     <t>gesamtes Colon</t>
   </si>
   <si>
@@ -146,48 +113,15 @@
     <t>keine Blutung</t>
   </si>
   <si>
-    <t>sickernd</t>
-  </si>
-  <si>
-    <t>spritzend, arteriell</t>
-  </si>
-  <si>
-    <t>spritzend, arteriell;spritzend arteriell</t>
-  </si>
-  <si>
-    <t>Empfehlung</t>
-  </si>
-  <si>
-    <t>Wiedervorstellung</t>
-  </si>
-  <si>
-    <t>Kontrolluntersuchung</t>
-  </si>
-  <si>
-    <t>keine weitere Empfehlung</t>
-  </si>
-  <si>
-    <t>mit Einengung</t>
-  </si>
-  <si>
     <t>ohne Einengung</t>
   </si>
   <si>
-    <t>mit Einengung;mit Lumeneinengung</t>
-  </si>
-  <si>
     <t>ohne Einengung;ohne Lumeneinengung</t>
   </si>
   <si>
     <t>Colon descendens;Kolon descendens;Colon desc</t>
   </si>
   <si>
-    <t>OP allgemein</t>
-  </si>
-  <si>
-    <t>OP zur Blutstillung</t>
-  </si>
-  <si>
     <t>Colon descendens</t>
   </si>
   <si>
@@ -215,39 +149,15 @@
     <t>Ausschluss Befund</t>
   </si>
   <si>
-    <t>CG7</t>
-  </si>
-  <si>
-    <t>CG8</t>
-  </si>
-  <si>
-    <t>CG9</t>
-  </si>
-  <si>
     <t>CG10</t>
   </si>
   <si>
-    <t>CG11</t>
-  </si>
-  <si>
     <t>Variable-Synonyme</t>
   </si>
   <si>
     <t>\n\nDivertikulose\n</t>
   </si>
   <si>
-    <t>Divertikulose Beschreibung: Mit einzelnen Divertikeln. \n</t>
-  </si>
-  <si>
-    <t>Divertikulose Beschreibung: Mit mehreren Divertikeln. \n</t>
-  </si>
-  <si>
-    <t>Divertikulose Beschreibung: Mit vielen Divertikeln. \n</t>
-  </si>
-  <si>
-    <t>Divertikulose Beschreibung: Mit vielen großen Divertikeln. \n</t>
-  </si>
-  <si>
     <t>Hauptlokalisation im gesamten Colon. \n</t>
   </si>
   <si>
@@ -275,34 +185,94 @@
     <t>Hauptlokalisation vor allem im Bereich des Coecums. \n</t>
   </si>
   <si>
-    <t>Divertikulose mit Lumeneinengung. \n</t>
-  </si>
-  <si>
     <t>Divertikulose ohne Lumeneinengung. \n</t>
   </si>
   <si>
     <t>Es gibt keine Blutung. \n</t>
   </si>
   <si>
-    <t>Es gibt eine sickernde Divertikelblutung. \n</t>
-  </si>
-  <si>
-    <t>Es gibt eine spritzend, arterielle Divertikelblutung. \n</t>
-  </si>
-  <si>
-    <t>Eine OP sollte erfolgen. \n</t>
-  </si>
-  <si>
-    <t>Eine OP zur Blutstillung sollte erfolgen. \n</t>
-  </si>
-  <si>
-    <t>Es sollte eine Wiedervorstellung stattfinden. \n</t>
-  </si>
-  <si>
-    <t>Es sollte eine Kontrolluntersuchung stattfinden. \n</t>
-  </si>
-  <si>
-    <t>Ansonsten keine weitere Empfehlung. \n</t>
+    <t>vorhanden</t>
+  </si>
+  <si>
+    <t>Blutung vorhanden</t>
+  </si>
+  <si>
+    <t>Es gibt eine Divertikelblutung. \n</t>
+  </si>
+  <si>
+    <t>Lokalisation</t>
+  </si>
+  <si>
+    <t>Ausprägung</t>
+  </si>
+  <si>
+    <t>einzeln</t>
+  </si>
+  <si>
+    <t>mehrere</t>
+  </si>
+  <si>
+    <t>viele</t>
+  </si>
+  <si>
+    <t>viele und große</t>
+  </si>
+  <si>
+    <t>CG1</t>
+  </si>
+  <si>
+    <t>CG2</t>
+  </si>
+  <si>
+    <t>CG3</t>
+  </si>
+  <si>
+    <t>kurzstreckig, passierbar</t>
+  </si>
+  <si>
+    <t>längerstreckig, passierbar</t>
+  </si>
+  <si>
+    <t>V.a. Verwachsungen</t>
+  </si>
+  <si>
+    <t>vor allem Verwachsungen</t>
+  </si>
+  <si>
+    <t>nicht passierbar</t>
+  </si>
+  <si>
+    <t>LE51</t>
+  </si>
+  <si>
+    <t>Zahl</t>
+  </si>
+  <si>
+    <t>bei ... cm</t>
+  </si>
+  <si>
+    <t>Ausprägung einzeln.\n</t>
+  </si>
+  <si>
+    <t>Mehrere Ausprägungen.\n</t>
+  </si>
+  <si>
+    <t>Viele Ausprägungen.\n</t>
+  </si>
+  <si>
+    <t>Viele und große Ausprägungen.\n</t>
+  </si>
+  <si>
+    <t>Divertikulose mit kurzstreckiger, passierbarer Lumeneinengung. \n</t>
+  </si>
+  <si>
+    <t>Divertikulose mit langstreckiger, passierbarer Lumeneinengung. \n</t>
+  </si>
+  <si>
+    <t>Divertikulose mit v.a. Verwachsungen.\n</t>
+  </si>
+  <si>
+    <t>Divertikulose mit nicht passierbarer Lumeneinengung bei %LE51% cm.\n</t>
   </si>
 </sst>
 </file>
@@ -671,12 +641,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:X191"/>
+  <dimension ref="A1:W193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,24 +656,23 @@
     <col min="3" max="3" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.6328125" customWidth="1"/>
     <col min="5" max="5" width="94.81640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" customWidth="1"/>
-    <col min="8" max="8" width="26" style="3" customWidth="1"/>
+    <col min="6" max="6" width="4.90625" customWidth="1"/>
+    <col min="7" max="7" width="4.1796875" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" style="3" customWidth="1"/>
     <col min="9" max="9" width="6.453125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="6.453125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="4.7265625" style="3" customWidth="1"/>
     <col min="12" max="12" width="22.90625" customWidth="1"/>
-    <col min="13" max="13" width="32.08984375" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" customWidth="1"/>
     <col min="14" max="14" width="35.6328125" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="11.6328125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="21.36328125" style="3" customWidth="1"/>
     <col min="17" max="17" width="59.90625" customWidth="1"/>
     <col min="18" max="18" width="102.1796875" customWidth="1"/>
-    <col min="19" max="19" width="37.6328125" customWidth="1"/>
-    <col min="20" max="1027" width="10.453125" customWidth="1"/>
+    <col min="19" max="1026" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,13 +680,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -726,16 +695,16 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
         <v>5</v>
@@ -750,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="Q1" t="s">
         <v>9</v>
@@ -761,110 +730,96 @@
       <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2" s="3"/>
       <c r="R2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B3"/>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
       <c r="H3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="I3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="Q3"/>
+      <c r="R3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L4" s="3"/>
       <c r="R4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5"/>
-      <c r="B5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5"/>
+        <v>29</v>
+      </c>
       <c r="H5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="Q5"/>
+        <v>62</v>
+      </c>
+      <c r="L5" s="3"/>
       <c r="R5" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L6" s="3"/>
       <c r="R6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7"/>
       <c r="B7"/>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="3" t="s">
         <v>62</v>
@@ -875,48 +830,47 @@
       <c r="O7"/>
       <c r="Q7"/>
       <c r="R7" t="s">
-        <v>72</v>
-      </c>
-      <c r="S7"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>62</v>
       </c>
       <c r="L8" s="3"/>
       <c r="R8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>62</v>
       </c>
       <c r="L9" s="3"/>
       <c r="R9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -929,279 +883,225 @@
       <c r="O10"/>
       <c r="Q10"/>
       <c r="R10" t="s">
-        <v>75</v>
-      </c>
-      <c r="S10"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="L11" s="3"/>
       <c r="R11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R15" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="R12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
-      <c r="Q13"/>
-      <c r="R13" t="s">
-        <v>78</v>
-      </c>
-      <c r="S13"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="R14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D15" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
         <v>17</v>
       </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" s="3"/>
-      <c r="R15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L16" s="3"/>
       <c r="R16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
+        <v>65</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L17" s="3"/>
       <c r="R17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" t="s">
-        <v>18</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="R18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
+      <c r="R18" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="3"/>
-      <c r="R19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
+      <c r="R19" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L20" s="3"/>
-      <c r="R20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="L20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="L21" s="3"/>
       <c r="R21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="L22" s="3"/>
       <c r="R22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L23" s="3"/>
-      <c r="R23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>65</v>
-      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L24" s="3"/>
-      <c r="R24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>65</v>
-      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L25" s="3"/>
-      <c r="R25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="1"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
@@ -1209,7 +1109,7 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
@@ -1217,139 +1117,147 @@
       <c r="Q29" s="3"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="Q30" s="3"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="Q31" s="3"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32" s="3"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32" s="3"/>
-      <c r="I32"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L32" s="3"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32" s="3"/>
-      <c r="Q32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
+      <c r="R32" s="1"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L33" s="3"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34" s="3"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34" s="3"/>
+      <c r="I34"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34" s="3"/>
+      <c r="Q34"/>
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="4"/>
       <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L37" s="3"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L38" s="3"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L39" s="3"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L40" s="3"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-    </row>
-    <row r="42" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-    </row>
-    <row r="43" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L41" s="3"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L42" s="3"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="R44" s="1"/>
-    </row>
-    <row r="45" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="R45" s="4"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+    </row>
+    <row r="45" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-    </row>
-    <row r="47" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="R46" s="1"/>
+    </row>
+    <row r="47" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="R47" s="4"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="E48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
     <row r="49" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="E50" s="3"/>
       <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
     </row>
     <row r="51" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="L52" s="3"/>
     </row>
     <row r="53" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M55"/>
-      <c r="N55"/>
-      <c r="O55"/>
-    </row>
-    <row r="56" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="L57" s="3"/>
-      <c r="R57" s="1"/>
-    </row>
-    <row r="58" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="L54" s="3"/>
+    </row>
+    <row r="55" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+    </row>
+    <row r="58" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E58" s="3"/>
+    </row>
     <row r="59" spans="4:18" x14ac:dyDescent="0.35">
       <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="L60" s="3"/>
-    </row>
+      <c r="R59" s="1"/>
+    </row>
+    <row r="60" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="4:18" x14ac:dyDescent="0.35">
       <c r="L61" s="3"/>
     </row>
@@ -1368,79 +1276,78 @@
     <row r="66" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L66" s="3"/>
     </row>
-    <row r="69" spans="12:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D96" s="3"/>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="67" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L67" s="3"/>
+    </row>
+    <row r="68" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L68" s="3"/>
+    </row>
+    <row r="71" spans="12:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106" s="3"/>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D106" s="3"/>
-      <c r="E106"/>
-      <c r="F106"/>
-      <c r="G106"/>
-      <c r="H106" s="3"/>
-      <c r="I106"/>
-      <c r="J106" s="3"/>
-      <c r="K106" s="3"/>
-      <c r="L106"/>
-      <c r="M106"/>
-      <c r="N106"/>
-      <c r="O106"/>
-      <c r="P106" s="3"/>
-      <c r="Q106"/>
-      <c r="R106"/>
-      <c r="S106"/>
-      <c r="T106"/>
-      <c r="U106"/>
-      <c r="V106"/>
-      <c r="W106"/>
-      <c r="X106"/>
-    </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A108"/>
+      <c r="B108"/>
+      <c r="C108" s="3"/>
       <c r="D108" s="3"/>
-    </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="E108"/>
+      <c r="F108"/>
+      <c r="G108"/>
+      <c r="H108" s="3"/>
+      <c r="I108"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108"/>
+      <c r="M108"/>
+      <c r="N108"/>
+      <c r="O108"/>
+      <c r="P108" s="3"/>
+      <c r="Q108"/>
+      <c r="R108"/>
+      <c r="S108"/>
+      <c r="T108"/>
+      <c r="U108"/>
+      <c r="V108"/>
+      <c r="W108"/>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.35">
@@ -1679,6 +1586,12 @@
     </row>
     <row r="191" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D191" s="3"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D193" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
excelparser: fixed synonym-parsing if synonyms is left empty and fixed errors in endo templates
</commit_message>
<xml_diff>
--- a/Schablonen/Divertikulose.xlsx
+++ b/Schablonen/Divertikulose.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FE9ADF-DE29-435A-BC43-4DBF54BBEBC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75913A82-BB3A-41C2-9293-0EE4D0B07D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="41180" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6420" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Textbausteine befundeingabestru" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>Gliederung</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Variable-Synonyme</t>
   </si>
   <si>
-    <t>\n\nDivertikulose\n</t>
-  </si>
-  <si>
     <t>Hauptlokalisation im gesamten Colon. \n</t>
   </si>
   <si>
@@ -273,6 +270,18 @@
   </si>
   <si>
     <t>Divertikulose mit nicht passierbarer Lumeneinengung bei %LE51% cm.\n</t>
+  </si>
+  <si>
+    <t>Divertikulose\n</t>
+  </si>
+  <si>
+    <t>\n\nAusprägung:\n</t>
+  </si>
+  <si>
+    <t>\n\nLumeneinengung:\n</t>
+  </si>
+  <si>
+    <t>\n\nBlutung:\n</t>
   </si>
 </sst>
 </file>
@@ -641,12 +650,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:W193"/>
+  <dimension ref="A1:W196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
+      <selection pane="bottomLeft" activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,12 +746,12 @@
       </c>
       <c r="L2" s="3"/>
       <c r="R2" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3"/>
       <c r="D3" t="s">
@@ -754,7 +763,7 @@
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I3"/>
       <c r="M3"/>
@@ -762,7 +771,7 @@
       <c r="O3"/>
       <c r="Q3"/>
       <c r="R3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
@@ -773,11 +782,11 @@
         <v>13</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L4" s="3"/>
       <c r="R4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -788,11 +797,11 @@
         <v>29</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" s="3"/>
       <c r="R5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -803,11 +812,11 @@
         <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" s="3"/>
       <c r="R6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -822,7 +831,7 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7"/>
       <c r="M7"/>
@@ -830,7 +839,7 @@
       <c r="O7"/>
       <c r="Q7"/>
       <c r="R7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
@@ -841,11 +850,11 @@
         <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8" s="3"/>
       <c r="R8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -856,11 +865,11 @@
         <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" s="3"/>
       <c r="R9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -875,7 +884,7 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I10"/>
       <c r="M10"/>
@@ -883,7 +892,7 @@
       <c r="O10"/>
       <c r="Q10"/>
       <c r="R10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -897,203 +906,218 @@
         <v>17</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L11" s="3"/>
       <c r="R11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R15" s="3" t="s">
+      <c r="L18" s="3"/>
+      <c r="R18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="R19" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16" s="3"/>
-      <c r="R16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="3"/>
-      <c r="R17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="R22" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>26</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E24" t="s">
         <v>26</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F24" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="3"/>
-      <c r="R21" t="s">
+      <c r="L24" s="3"/>
+      <c r="R24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="D22" t="s">
+      <c r="E25" t="s">
         <v>53</v>
       </c>
-      <c r="E22" t="s">
+      <c r="H25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="3"/>
+      <c r="R25" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22" s="3"/>
-      <c r="R22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L26" s="3"/>
@@ -1103,27 +1127,12 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L31" s="3"/>
@@ -1135,138 +1144,153 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="Q32" s="3"/>
       <c r="R32" s="1"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="Q33" s="3"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34" s="3"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34" s="3"/>
-      <c r="I34"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L34" s="3"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34" s="3"/>
-      <c r="Q34"/>
-      <c r="S34"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="1"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="R35" s="1"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="4"/>
       <c r="L36" s="3"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37" s="3"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37" s="3"/>
+      <c r="I37"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
       <c r="L37" s="3"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37" s="3"/>
+      <c r="Q37"/>
+      <c r="S37"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="L38" s="3"/>
+      <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="4"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L40" s="3"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L41" s="3"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="L42" s="3"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-    </row>
-    <row r="44" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-    </row>
-    <row r="45" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="R46" s="1"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L43" s="3"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L44" s="3"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L45" s="3"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
     </row>
     <row r="47" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="R47" s="4"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-    </row>
-    <row r="49" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-    </row>
-    <row r="51" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="E52" s="3"/>
-      <c r="L52" s="3"/>
-    </row>
-    <row r="53" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="L54" s="3"/>
-    </row>
-    <row r="55" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+    </row>
+    <row r="48" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+    </row>
+    <row r="49" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="R50" s="4"/>
+    </row>
+    <row r="51" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+    </row>
+    <row r="52" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+    </row>
+    <row r="54" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="E55" s="3"/>
+      <c r="L55" s="3"/>
+    </row>
     <row r="56" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="M57"/>
-      <c r="N57"/>
-      <c r="O57"/>
-    </row>
-    <row r="58" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="L59" s="3"/>
-      <c r="R59" s="1"/>
-    </row>
-    <row r="60" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="4:18" x14ac:dyDescent="0.35">
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+    </row>
     <row r="61" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="L61" s="3"/>
+      <c r="E61" s="3"/>
     </row>
     <row r="62" spans="4:18" x14ac:dyDescent="0.35">
       <c r="L62" s="3"/>
-    </row>
-    <row r="63" spans="4:18" x14ac:dyDescent="0.35">
-      <c r="L63" s="3"/>
-    </row>
+      <c r="R62" s="1"/>
+    </row>
+    <row r="63" spans="4:18" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="4:18" x14ac:dyDescent="0.35">
       <c r="L64" s="3"/>
     </row>
@@ -1282,16 +1306,16 @@
     <row r="68" spans="12:12" x14ac:dyDescent="0.35">
       <c r="L68" s="3"/>
     </row>
-    <row r="71" spans="12:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="D98" s="3"/>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="D99" s="3"/>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="D100" s="3"/>
-    </row>
+    <row r="69" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L69" s="3"/>
+    </row>
+    <row r="70" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L70" s="3"/>
+    </row>
+    <row r="71" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L71" s="3"/>
+    </row>
+    <row r="74" spans="12:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D101" s="3"/>
     </row>
@@ -1313,30 +1337,8 @@
     <row r="107" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="C108" s="3"/>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D108" s="3"/>
-      <c r="E108"/>
-      <c r="F108"/>
-      <c r="G108"/>
-      <c r="H108" s="3"/>
-      <c r="I108"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108"/>
-      <c r="M108"/>
-      <c r="N108"/>
-      <c r="O108"/>
-      <c r="P108" s="3"/>
-      <c r="Q108"/>
-      <c r="R108"/>
-      <c r="S108"/>
-      <c r="T108"/>
-      <c r="U108"/>
-      <c r="V108"/>
-      <c r="W108"/>
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D109" s="3"/>
@@ -1344,8 +1346,30 @@
     <row r="110" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A111"/>
+      <c r="B111"/>
+      <c r="C111" s="3"/>
       <c r="D111" s="3"/>
+      <c r="E111"/>
+      <c r="F111"/>
+      <c r="G111"/>
+      <c r="H111" s="3"/>
+      <c r="I111"/>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+      <c r="P111" s="3"/>
+      <c r="Q111"/>
+      <c r="R111"/>
+      <c r="S111"/>
+      <c r="T111"/>
+      <c r="U111"/>
+      <c r="V111"/>
+      <c r="W111"/>
     </row>
     <row r="112" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D112" s="3"/>
@@ -1592,6 +1616,15 @@
     </row>
     <row r="193" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D193" s="3"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D196" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>